<commit_message>
Adds train test xlsx
</commit_message>
<xml_diff>
--- a/notebooks/aggregated_results/correct_results.xlsx
+++ b/notebooks/aggregated_results/correct_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>total_correct</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>tag</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -515,6 +520,9 @@
       </c>
       <c r="J2" t="n">
         <v>4</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -548,6 +556,9 @@
       <c r="J3" t="n">
         <v>4</v>
       </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -576,6 +587,9 @@
       <c r="J4" t="n">
         <v>4</v>
       </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -608,6 +622,9 @@
       <c r="J5" t="n">
         <v>7</v>
       </c>
+      <c r="K5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -640,6 +657,9 @@
       <c r="J6" t="n">
         <v>4</v>
       </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -672,6 +692,9 @@
       <c r="J7" t="n">
         <v>4</v>
       </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -704,6 +727,9 @@
       <c r="J8" t="n">
         <v>6</v>
       </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -731,6 +757,9 @@
       </c>
       <c r="J9" t="n">
         <v>4</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -758,6 +787,9 @@
       <c r="J10" t="n">
         <v>4</v>
       </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -790,6 +822,9 @@
       <c r="J11" t="n">
         <v>4</v>
       </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -822,6 +857,9 @@
       <c r="J12" t="n">
         <v>5</v>
       </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -854,6 +892,9 @@
       <c r="J13" t="n">
         <v>5</v>
       </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -886,6 +927,9 @@
       <c r="J14" t="n">
         <v>5</v>
       </c>
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -918,6 +962,9 @@
       <c r="J15" t="n">
         <v>4</v>
       </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -950,6 +997,9 @@
       <c r="J16" t="n">
         <v>6</v>
       </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -982,6 +1032,9 @@
       <c r="J17" t="n">
         <v>6</v>
       </c>
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1014,6 +1067,9 @@
       <c r="J18" t="n">
         <v>3</v>
       </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1041,6 +1097,9 @@
       </c>
       <c r="J19" t="n">
         <v>4</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1068,6 +1127,9 @@
       <c r="J20" t="n">
         <v>4</v>
       </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1100,6 +1162,9 @@
       <c r="J21" t="n">
         <v>5</v>
       </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1132,6 +1197,9 @@
       <c r="J22" t="n">
         <v>2</v>
       </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1164,6 +1232,9 @@
       <c r="J23" t="n">
         <v>3</v>
       </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1195,6 +1266,9 @@
       </c>
       <c r="J24" t="n">
         <v>3</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1222,6 +1296,9 @@
       <c r="J25" t="n">
         <v>4</v>
       </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1254,6 +1331,9 @@
       <c r="J26" t="n">
         <v>5</v>
       </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1284,6 +1364,9 @@
       <c r="J27" t="n">
         <v>3</v>
       </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1312,6 +1395,9 @@
       <c r="J28" t="n">
         <v>3</v>
       </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1344,6 +1430,9 @@
       <c r="J29" t="n">
         <v>6</v>
       </c>
+      <c r="K29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1376,6 +1465,9 @@
       <c r="J30" t="n">
         <v>5</v>
       </c>
+      <c r="K30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1408,6 +1500,9 @@
       <c r="J31" t="n">
         <v>4</v>
       </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1440,6 +1535,9 @@
       <c r="J32" t="n">
         <v>3</v>
       </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1472,6 +1570,9 @@
       <c r="J33" t="n">
         <v>2</v>
       </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1504,6 +1605,9 @@
       <c r="J34" t="n">
         <v>8</v>
       </c>
+      <c r="K34" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1536,6 +1640,9 @@
       <c r="J35" t="n">
         <v>7</v>
       </c>
+      <c r="K35" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1568,6 +1675,9 @@
       <c r="J36" t="n">
         <v>7</v>
       </c>
+      <c r="K36" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1595,6 +1705,9 @@
       </c>
       <c r="J37" t="n">
         <v>4</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1620,6 +1733,9 @@
       <c r="J38" t="n">
         <v>3</v>
       </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1652,6 +1768,9 @@
       <c r="J39" t="n">
         <v>4</v>
       </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1684,6 +1803,9 @@
       <c r="J40" t="n">
         <v>6</v>
       </c>
+      <c r="K40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1716,6 +1838,9 @@
       <c r="J41" t="n">
         <v>3</v>
       </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1748,6 +1873,9 @@
       <c r="J42" t="n">
         <v>4</v>
       </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1776,6 +1904,9 @@
       <c r="J43" t="n">
         <v>4</v>
       </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1808,6 +1939,9 @@
       <c r="J44" t="n">
         <v>6</v>
       </c>
+      <c r="K44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1840,6 +1974,9 @@
       <c r="J45" t="n">
         <v>4</v>
       </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1872,6 +2009,9 @@
       <c r="J46" t="n">
         <v>6</v>
       </c>
+      <c r="K46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1904,6 +2044,9 @@
       <c r="J47" t="n">
         <v>4</v>
       </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1936,6 +2079,9 @@
       <c r="J48" t="n">
         <v>7</v>
       </c>
+      <c r="K48" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1968,6 +2114,9 @@
       <c r="J49" t="n">
         <v>6</v>
       </c>
+      <c r="K49" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2000,6 +2149,9 @@
       <c r="J50" t="n">
         <v>5</v>
       </c>
+      <c r="K50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2028,6 +2180,9 @@
       <c r="J51" t="n">
         <v>4</v>
       </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2060,6 +2215,9 @@
       <c r="J52" t="n">
         <v>6</v>
       </c>
+      <c r="K52" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2092,6 +2250,9 @@
       <c r="J53" t="n">
         <v>7</v>
       </c>
+      <c r="K53" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2124,6 +2285,9 @@
       <c r="J54" t="n">
         <v>5</v>
       </c>
+      <c r="K54" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2156,6 +2320,9 @@
       <c r="J55" t="n">
         <v>5</v>
       </c>
+      <c r="K55" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2188,6 +2355,9 @@
       <c r="J56" t="n">
         <v>7</v>
       </c>
+      <c r="K56" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2220,6 +2390,9 @@
       <c r="J57" t="n">
         <v>6</v>
       </c>
+      <c r="K57" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -2252,6 +2425,9 @@
       <c r="J58" t="n">
         <v>7</v>
       </c>
+      <c r="K58" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -2284,6 +2460,9 @@
       <c r="J59" t="n">
         <v>8</v>
       </c>
+      <c r="K59" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2316,6 +2495,9 @@
       <c r="J60" t="n">
         <v>6</v>
       </c>
+      <c r="K60" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2348,6 +2530,9 @@
       <c r="J61" t="n">
         <v>6</v>
       </c>
+      <c r="K61" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2380,6 +2565,9 @@
       <c r="J62" t="n">
         <v>3</v>
       </c>
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2412,6 +2600,9 @@
       <c r="J63" t="n">
         <v>7</v>
       </c>
+      <c r="K63" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2444,6 +2635,9 @@
       <c r="J64" t="n">
         <v>7</v>
       </c>
+      <c r="K64" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -2476,6 +2670,9 @@
       <c r="J65" t="n">
         <v>8</v>
       </c>
+      <c r="K65" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2508,6 +2705,9 @@
       <c r="J66" t="n">
         <v>7</v>
       </c>
+      <c r="K66" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -2540,6 +2740,9 @@
       <c r="J67" t="n">
         <v>7</v>
       </c>
+      <c r="K67" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -2572,6 +2775,9 @@
       <c r="J68" t="n">
         <v>5</v>
       </c>
+      <c r="K68" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -2603,6 +2809,9 @@
       </c>
       <c r="J69" t="n">
         <v>6</v>
+      </c>
+      <c r="K69" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2626,6 +2835,9 @@
       <c r="J70" t="n">
         <v>1</v>
       </c>
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -2658,6 +2870,9 @@
       <c r="J71" t="n">
         <v>7</v>
       </c>
+      <c r="K71" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -2690,6 +2905,9 @@
       <c r="J72" t="n">
         <v>4</v>
       </c>
+      <c r="K72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -2722,6 +2940,9 @@
       <c r="J73" t="n">
         <v>5</v>
       </c>
+      <c r="K73" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -2754,6 +2975,9 @@
       <c r="J74" t="n">
         <v>6</v>
       </c>
+      <c r="K74" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -2786,6 +3010,9 @@
       <c r="J75" t="n">
         <v>6</v>
       </c>
+      <c r="K75" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -2818,6 +3045,9 @@
       <c r="J76" t="n">
         <v>7</v>
       </c>
+      <c r="K76" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -2850,6 +3080,9 @@
       <c r="J77" t="n">
         <v>5</v>
       </c>
+      <c r="K77" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -2882,6 +3115,9 @@
       <c r="J78" t="n">
         <v>5</v>
       </c>
+      <c r="K78" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -2912,6 +3148,9 @@
       <c r="J79" t="n">
         <v>4</v>
       </c>
+      <c r="K79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -2944,6 +3183,9 @@
       <c r="J80" t="n">
         <v>3</v>
       </c>
+      <c r="K80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -2976,6 +3218,9 @@
       <c r="J81" t="n">
         <v>4</v>
       </c>
+      <c r="K81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -3008,6 +3253,9 @@
       <c r="J82" t="n">
         <v>5</v>
       </c>
+      <c r="K82" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -3040,6 +3288,9 @@
       <c r="J83" t="n">
         <v>4</v>
       </c>
+      <c r="K83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -3070,6 +3321,9 @@
       <c r="J84" t="n">
         <v>5</v>
       </c>
+      <c r="K84" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -3102,6 +3356,9 @@
       <c r="J85" t="n">
         <v>5</v>
       </c>
+      <c r="K85" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -3134,6 +3391,9 @@
       <c r="J86" t="n">
         <v>7</v>
       </c>
+      <c r="K86" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -3166,6 +3426,9 @@
       <c r="J87" t="n">
         <v>6</v>
       </c>
+      <c r="K87" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -3198,6 +3461,9 @@
       <c r="J88" t="n">
         <v>6</v>
       </c>
+      <c r="K88" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -3230,6 +3496,9 @@
       <c r="J89" t="n">
         <v>7</v>
       </c>
+      <c r="K89" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3260,6 +3529,9 @@
       <c r="J90" t="n">
         <v>6</v>
       </c>
+      <c r="K90" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -3292,6 +3564,9 @@
       <c r="J91" t="n">
         <v>4</v>
       </c>
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -3324,6 +3599,9 @@
       <c r="J92" t="n">
         <v>4</v>
       </c>
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -3356,6 +3634,9 @@
       <c r="J93" t="n">
         <v>4</v>
       </c>
+      <c r="K93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -3388,6 +3669,9 @@
       <c r="J94" t="n">
         <v>3</v>
       </c>
+      <c r="K94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -3420,6 +3704,9 @@
       <c r="J95" t="n">
         <v>4</v>
       </c>
+      <c r="K95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -3452,6 +3739,9 @@
       <c r="J96" t="n">
         <v>8</v>
       </c>
+      <c r="K96" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -3484,6 +3774,9 @@
       <c r="J97" t="n">
         <v>7</v>
       </c>
+      <c r="K97" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -3516,6 +3809,9 @@
       <c r="J98" t="n">
         <v>6</v>
       </c>
+      <c r="K98" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -3548,6 +3844,9 @@
       <c r="J99" t="n">
         <v>7</v>
       </c>
+      <c r="K99" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -3580,6 +3879,9 @@
       <c r="J100" t="n">
         <v>7</v>
       </c>
+      <c r="K100" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -3611,6 +3913,9 @@
       </c>
       <c r="J101" t="n">
         <v>5</v>
+      </c>
+      <c r="K101" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>